<commit_message>
Se modifican los archivos para el EDA
</commit_message>
<xml_diff>
--- a/outputs/eda/EDA_informe.xlsx
+++ b/outputs/eda/EDA_informe.xlsx
@@ -10,18 +10,13 @@
     <sheet name="EURUSD_HEAD" sheetId="1" r:id="rId1"/>
     <sheet name="EURUSD_RESUMEN" sheetId="2" r:id="rId2"/>
     <sheet name="EURUSD_STATS" sheetId="3" r:id="rId3"/>
-    <sheet name="US500_HEAD" sheetId="4" r:id="rId4"/>
-    <sheet name="US500_RESUMEN" sheetId="5" r:id="rId5"/>
-    <sheet name="US500_STATS" sheetId="6" r:id="rId6"/>
-    <sheet name="Correlation_matrix" sheetId="7" r:id="rId7"/>
-    <sheet name="Rolling_corr" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Open</t>
   </si>
@@ -38,7 +33,7 @@
     <t>Volume</t>
   </si>
   <si>
-    <t>timestamp</t>
+    <t>Date</t>
   </si>
   <si>
     <t>activo</t>
@@ -93,18 +88,6 @@
   </si>
   <si>
     <t>ES_95</t>
-  </si>
-  <si>
-    <t>US500</t>
-  </si>
-  <si>
-    <t>lr_EURUSD</t>
-  </si>
-  <si>
-    <t>lr_US500</t>
-  </si>
-  <si>
-    <t>rolling_corr</t>
   </si>
 </sst>
 </file>
@@ -497,102 +480,102 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45912</v>
+        <v>43118</v>
       </c>
       <c r="B2">
-        <v>1.17245</v>
+        <v>1.21844</v>
       </c>
       <c r="C2">
-        <v>1.17472</v>
+        <v>1.22646</v>
       </c>
       <c r="D2">
-        <v>1.17009</v>
+        <v>1.21646</v>
       </c>
       <c r="E2">
-        <v>1.17316</v>
+        <v>1.2239</v>
       </c>
       <c r="F2">
-        <v>33188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45915</v>
+        <v>43119</v>
       </c>
       <c r="B3">
-        <v>1.17293</v>
+        <v>1.22373</v>
       </c>
       <c r="C3">
-        <v>1.17739</v>
+        <v>1.22951</v>
       </c>
       <c r="D3">
-        <v>1.17158</v>
+        <v>1.22145</v>
       </c>
       <c r="E3">
-        <v>1.17602</v>
+        <v>1.22157</v>
       </c>
       <c r="F3">
-        <v>33278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45916</v>
+        <v>43122</v>
       </c>
       <c r="B4">
-        <v>1.17602</v>
+        <v>1.22695</v>
       </c>
       <c r="C4">
-        <v>1.18778</v>
+        <v>1.22722</v>
       </c>
       <c r="D4">
-        <v>1.17569</v>
+        <v>1.22137</v>
       </c>
       <c r="E4">
-        <v>1.1865</v>
+        <v>1.22616</v>
       </c>
       <c r="F4">
-        <v>53413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45917</v>
+        <v>43123</v>
       </c>
       <c r="B5">
-        <v>1.18532</v>
+        <v>1.22606</v>
       </c>
       <c r="C5">
-        <v>1.19183</v>
+        <v>1.23062</v>
       </c>
       <c r="D5">
-        <v>1.18075</v>
+        <v>1.22228</v>
       </c>
       <c r="E5">
-        <v>1.18117</v>
+        <v>1.22979</v>
       </c>
       <c r="F5">
-        <v>58996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45918</v>
+        <v>43124</v>
       </c>
       <c r="B6">
-        <v>1.18102</v>
+        <v>1.22983</v>
       </c>
       <c r="C6">
-        <v>1.18478</v>
+        <v>1.24147</v>
       </c>
       <c r="D6">
-        <v>1.17494</v>
+        <v>1.229</v>
       </c>
       <c r="E6">
-        <v>1.17819</v>
+        <v>1.24069</v>
       </c>
       <c r="F6">
-        <v>62294</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -639,25 +622,25 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>2000</v>
       </c>
       <c r="C2" s="3">
-        <v>45912</v>
+        <v>43118</v>
       </c>
       <c r="D2" s="3">
-        <v>45923</v>
+        <v>45931</v>
       </c>
       <c r="E2">
-        <v>1.18003</v>
+        <v>1.17359</v>
       </c>
       <c r="F2">
-        <v>1.17868875</v>
+        <v>1.1195519</v>
       </c>
       <c r="G2">
-        <v>1.17316</v>
+        <v>0.95906</v>
       </c>
       <c r="H2">
-        <v>1.1865</v>
+        <v>1.25068</v>
       </c>
     </row>
   </sheetData>
@@ -704,364 +687,31 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>7</v>
+        <v>1999</v>
       </c>
       <c r="B2">
-        <v>0.0008341284466841316</v>
+        <v>-2.099802620637938E-05</v>
       </c>
       <c r="C2">
-        <v>0.004864457513254942</v>
+        <v>0.004579851808568483</v>
       </c>
       <c r="D2">
-        <v>0.6728768687821665</v>
+        <v>0.09763861887018443</v>
       </c>
       <c r="E2">
-        <v>-0.6461914315423902</v>
+        <v>1.711949035004622</v>
       </c>
       <c r="F2">
-        <v>0.6174207361856244</v>
+        <v>245.2086556092065</v>
       </c>
       <c r="G2">
-        <v>0.7343934429998594</v>
+        <v>5.670442840525196E-54</v>
       </c>
       <c r="H2">
-        <v>-0.004143768107473594</v>
+        <v>-0.007311072280727136</v>
       </c>
       <c r="I2">
-        <v>-0.004502324229023053</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2">
-        <v>45910</v>
-      </c>
-      <c r="B2">
-        <v>6527.4</v>
-      </c>
-      <c r="C2">
-        <v>6538.6</v>
-      </c>
-      <c r="D2">
-        <v>6517.6</v>
-      </c>
-      <c r="E2">
-        <v>6532.5</v>
-      </c>
-      <c r="F2">
-        <v>8798</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2">
-        <v>45911</v>
-      </c>
-      <c r="B3">
-        <v>6541.3</v>
-      </c>
-      <c r="C3">
-        <v>6594.6</v>
-      </c>
-      <c r="D3">
-        <v>6531.9</v>
-      </c>
-      <c r="E3">
-        <v>6586.4</v>
-      </c>
-      <c r="F3">
-        <v>55282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>45912</v>
-      </c>
-      <c r="B4">
-        <v>6589.3</v>
-      </c>
-      <c r="C4">
-        <v>6607.1</v>
-      </c>
-      <c r="D4">
-        <v>6577.5</v>
-      </c>
-      <c r="E4">
-        <v>6589.7</v>
-      </c>
-      <c r="F4">
-        <v>49542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2">
-        <v>45915</v>
-      </c>
-      <c r="B5">
-        <v>6591.8</v>
-      </c>
-      <c r="C5">
-        <v>6626.4</v>
-      </c>
-      <c r="D5">
-        <v>6588.5</v>
-      </c>
-      <c r="E5">
-        <v>6620.6</v>
-      </c>
-      <c r="F5">
-        <v>63116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>45916</v>
-      </c>
-      <c r="B6">
-        <v>6624.6</v>
-      </c>
-      <c r="C6">
-        <v>6643.1</v>
-      </c>
-      <c r="D6">
-        <v>6607.8</v>
-      </c>
-      <c r="E6">
-        <v>6617.7</v>
-      </c>
-      <c r="F6">
-        <v>52484</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45910</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45923</v>
-      </c>
-      <c r="E2">
-        <v>6703.6</v>
-      </c>
-      <c r="F2">
-        <v>6626.780000000001</v>
-      </c>
-      <c r="G2">
-        <v>6532.5</v>
-      </c>
-      <c r="H2">
-        <v>6703.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>0.002872775235105528</v>
-      </c>
-      <c r="C2">
-        <v>0.003018128344315992</v>
-      </c>
-      <c r="D2">
-        <v>0.326043499749273</v>
-      </c>
-      <c r="E2">
-        <v>-0.6526362233126601</v>
-      </c>
-      <c r="F2">
-        <v>0.4417286218942582</v>
-      </c>
-      <c r="G2">
-        <v>0.8018254718479594</v>
-      </c>
-      <c r="H2">
-        <v>-0.0007285663877961923</v>
-      </c>
-      <c r="I2">
-        <v>-0.0009221954951978972</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>-0.07048369037270277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3">
-        <v>-0.07048369037270277</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>-0.009813679026569542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica el análisis exploratorio EDA, se agregan metricas de ARIMA y se agrega backtesting
</commit_message>
<xml_diff>
--- a/outputs/eda/EDA_informe.xlsx
+++ b/outputs/eda/EDA_informe.xlsx
@@ -12,9 +12,13 @@
     <sheet name="EURUSD_STATS" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="EURUSD_ARIMA_candidates" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="EURUSD_SARIMA_candidates" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="EURUSD_Narrative" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="EURUSD_Signals_guide" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Guide_columns" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Model_compare_summary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="EURUSD_Narrative" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="EURUSD_Signals_guide" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="EURUSD_DATA_QUALITY" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="EURUSD_STATIONARITY" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="EURUSD_Residuals_diag" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Guide_columns" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -484,19 +488,19 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
-        <v>43122</v>
+        <v>43123</v>
       </c>
       <c r="B2" t="n">
-        <v>1.22695</v>
+        <v>1.22606</v>
       </c>
       <c r="C2" t="n">
-        <v>1.22722</v>
+        <v>1.23062</v>
       </c>
       <c r="D2" t="n">
-        <v>1.22137</v>
+        <v>1.22228</v>
       </c>
       <c r="E2" t="n">
-        <v>1.22616</v>
+        <v>1.22979</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -504,19 +508,19 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="n">
-        <v>43123</v>
+        <v>43124</v>
       </c>
       <c r="B3" t="n">
-        <v>1.22606</v>
+        <v>1.22983</v>
       </c>
       <c r="C3" t="n">
-        <v>1.23062</v>
+        <v>1.24147</v>
       </c>
       <c r="D3" t="n">
-        <v>1.22228</v>
+        <v>1.229</v>
       </c>
       <c r="E3" t="n">
-        <v>1.22979</v>
+        <v>1.24069</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -524,19 +528,19 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
-        <v>43124</v>
+        <v>43125</v>
       </c>
       <c r="B4" t="n">
-        <v>1.22983</v>
+        <v>1.24071</v>
       </c>
       <c r="C4" t="n">
-        <v>1.24147</v>
+        <v>1.25376</v>
       </c>
       <c r="D4" t="n">
-        <v>1.229</v>
+        <v>1.23638</v>
       </c>
       <c r="E4" t="n">
-        <v>1.24069</v>
+        <v>1.23969</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -544,19 +548,19 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
-        <v>43125</v>
+        <v>43126</v>
       </c>
       <c r="B5" t="n">
-        <v>1.24071</v>
+        <v>1.23926</v>
       </c>
       <c r="C5" t="n">
-        <v>1.25376</v>
+        <v>1.24935</v>
       </c>
       <c r="D5" t="n">
-        <v>1.23638</v>
+        <v>1.23698</v>
       </c>
       <c r="E5" t="n">
-        <v>1.23969</v>
+        <v>1.24273</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -564,22 +568,662 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
-        <v>43126</v>
+        <v>43129</v>
       </c>
       <c r="B6" t="n">
-        <v>1.23926</v>
+        <v>1.24235</v>
       </c>
       <c r="C6" t="n">
-        <v>1.24935</v>
+        <v>1.2432</v>
       </c>
       <c r="D6" t="n">
-        <v>1.23698</v>
+        <v>1.23366</v>
       </c>
       <c r="E6" t="n">
-        <v>1.24273</v>
+        <v>1.23827</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>series</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>stat</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>lags_used</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>nobs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>crit_1%</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>crit_5%</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>crit_10%</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>conclusion</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>crit_2.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>EURUSD[level]</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ADF</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>-2.385964301215576</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1457371306121847</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1999</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-3.433625496286504</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2.862986937508278</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2.567540287745173</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>non-stationary</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>EURUSD[level]</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>KPSS</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2.035311725137694</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>28</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>0.739</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>non-stationary</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>0.574</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>EURUSD[Δlog]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ADF</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-44.3669005477752</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-3.433627137787501</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-2.862987662236822</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-2.56754067362658</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>stationary</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EURUSD[Δlog]</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>KPSS</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1766043103880247</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0.739</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>stationary</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0.574</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>lb_p_10</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>lb_p_20</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>modelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.9998647612658635</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9999999870973478</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ARIMA(3,1,1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sección</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Columna</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Significado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>p,d,q</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Órdenes no estacionales: AR (p), diferencias (d), MA (q).</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>bic</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Criterio de información bayesiano (menor es mejor).</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>aic</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Criterio de Akaike (menor es mejor).</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>lb_p</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>p-value de Ljung–Box en residuales (≥0.05 sugiere ruido blanco).</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>p,d,q</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Parte no estacional del modelo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>P,D,Q</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Parte estacional del modelo (lags a múltiplos de s).</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Periodo estacional (diario: 5=semana hábil, 7=semana).</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SARIMA_candidates</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>bic,aic,lb_p</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mismos criterios que en ARIMA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>STATS</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mean,std</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Media y desviación típica diaria de log-returns.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>STATS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>skew,kurtosis</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Asimetría y exceso de curtosis (colas).</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>STATS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JB_stat,JB_pvalue</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jarque–Bera (p&lt;0.05 ⇒ no normal).</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>STATS</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>VaR_95,ES_95</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Pérdida al 95% y pérdida media condicional en el 5% peor.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RESUMEN</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>precio_ultimo/promedio/min/max</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Niveles de precio del periodo resampleado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>RESUMEN</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>inicio,fin,filas</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Fechas de cobertura y nº de barras.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Signals_guide</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tendencia_MA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cruce SMA50 vs SMA200 (lectura descriptiva).</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Signals_guide</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RSI_14</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sobrecompra/sobreventa/neutral (14).</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Signals_guide</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MACD</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Relación MACD vs señal (12,26,9).</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Residuals_diag</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>lb_p_10, lb_p_20</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ljung–Box p-value en residuales (lags 10 y 20).</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Model_compare_summary</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ΔBIC_alt_vs_best</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Diferencia de BIC entre el alternativo y el recomendado (positivo=peor).</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -653,16 +1297,16 @@
         <v>2000</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>43122</v>
+        <v>43123</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>45933</v>
+        <v>45936</v>
       </c>
       <c r="E2" t="n">
-        <v>1.1739</v>
+        <v>1.17128</v>
       </c>
       <c r="F2" t="n">
-        <v>1.119501495</v>
+        <v>1.119474055</v>
       </c>
       <c r="G2" t="n">
         <v>0.95906</v>
@@ -742,22 +1386,22 @@
         <v>1999</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.178879229923747e-05</v>
+        <v>-2.438532025893065e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004579174566797649</v>
+        <v>0.004578956744010433</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09799270207228233</v>
+        <v>0.0995152332483944</v>
       </c>
       <c r="E2" t="n">
-        <v>1.714583104169098</v>
+        <v>1.715642934253303</v>
       </c>
       <c r="F2" t="n">
-        <v>245.978400364945</v>
+        <v>246.3792003493377</v>
       </c>
       <c r="G2" t="n">
-        <v>3.858948894252555e-54</v>
+        <v>3.158176635593929e-54</v>
       </c>
       <c r="H2" t="n">
         <v>-0.007311072280727136</v>
@@ -819,7 +1463,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -828,38 +1472,38 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-15813.29937544143</v>
+        <v>-15808.93391855776</v>
       </c>
       <c r="E2" t="n">
-        <v>-15835.69898327826</v>
+        <v>-15836.9334283538</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3020684463935297</v>
+        <v>0.4460986357228727</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
       <c r="D3" t="n">
-        <v>-15806.06524707452</v>
+        <v>-15771.5833113377</v>
       </c>
       <c r="E3" t="n">
-        <v>-15834.06475687056</v>
+        <v>-15805.18272309296</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3212411956801534</v>
+        <v>0.0008960997602847229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -868,18 +1512,18 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>-15799.94769439057</v>
+        <v>-15722.58449386945</v>
       </c>
       <c r="E4" t="n">
-        <v>-15833.54710614582</v>
+        <v>-15744.98410170628</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2422088242845229</v>
+        <v>8.99773815128505e-07</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -888,18 +1532,18 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>-15767.71324853276</v>
+        <v>-15687.65715511697</v>
       </c>
       <c r="E5" t="n">
-        <v>-15806.91256224722</v>
+        <v>-15715.65666491301</v>
       </c>
       <c r="F5" t="n">
-        <v>0.001551995392223732</v>
+        <v>9.057281081856922e-07</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -908,38 +1552,38 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>-15723.04301127229</v>
+        <v>-15661.53036690277</v>
       </c>
       <c r="E6" t="n">
-        <v>-15745.44261910913</v>
+        <v>-15700.72968061723</v>
       </c>
       <c r="F6" t="n">
-        <v>9.726585758003079e-07</v>
+        <v>1.544201155603525e-06</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>-15687.57860938746</v>
+        <v>-15650.35349427511</v>
       </c>
       <c r="E7" t="n">
-        <v>-15715.5781191835</v>
+        <v>-15667.15320015274</v>
       </c>
       <c r="F7" t="n">
-        <v>8.327443185526465e-07</v>
+        <v>8.88755867228312e-09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -948,18 +1592,18 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>-15650.76468296154</v>
+        <v>-15629.44824767751</v>
       </c>
       <c r="E8" t="n">
-        <v>-15667.56438883916</v>
+        <v>-15657.44775747356</v>
       </c>
       <c r="F8" t="n">
-        <v>9.205728464902888e-09</v>
+        <v>1.075416108568944e-08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -968,18 +1612,18 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>-15630.24200050064</v>
+        <v>-15626.22450793347</v>
       </c>
       <c r="E9" t="n">
-        <v>-15658.24151029669</v>
+        <v>-15648.62411577031</v>
       </c>
       <c r="F9" t="n">
-        <v>1.045251533727738e-08</v>
+        <v>6.62281654959856e-09</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -988,33 +1632,33 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>-15626.48481216527</v>
+        <v>-15608.86063372448</v>
       </c>
       <c r="E10" t="n">
-        <v>-15648.88442000211</v>
+        <v>-15642.46004547973</v>
       </c>
       <c r="F10" t="n">
-        <v>6.400591554488912e-09</v>
+        <v>3.798487396284246e-09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-15609.66599549213</v>
+        <v>-15551.64212938027</v>
       </c>
       <c r="E11" t="n">
-        <v>-15643.26540724738</v>
+        <v>-15574.0417372171</v>
       </c>
       <c r="F11" t="n">
-        <v>3.607492432460986e-09</v>
+        <v>2.896334386935552e-14</v>
       </c>
     </row>
   </sheetData>
@@ -1090,13 +1734,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -1111,13 +1755,13 @@
         <v>5</v>
       </c>
       <c r="H2" t="n">
-        <v>-14994.66042474442</v>
+        <v>-15004.99994700666</v>
       </c>
       <c r="I2" t="n">
-        <v>-15028.21159503376</v>
+        <v>-15032.96177764926</v>
       </c>
       <c r="J2" t="n">
-        <v>1.277413812049388e-40</v>
+        <v>3.43786698747402e-41</v>
       </c>
     </row>
     <row r="3">
@@ -1128,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -1143,18 +1787,18 @@
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>-14989.98408692264</v>
+        <v>-15002.94368122421</v>
       </c>
       <c r="I3" t="n">
-        <v>-15012.35556807402</v>
+        <v>-15030.90551186681</v>
       </c>
       <c r="J3" t="n">
-        <v>2.088417579977634e-46</v>
+        <v>2.371123554633866e-41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -1175,24 +1819,24 @@
         <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>-14985.4437259777</v>
+        <v>-14993.59098211363</v>
       </c>
       <c r="I4" t="n">
-        <v>-15024.58675798193</v>
+        <v>-15027.14215240297</v>
       </c>
       <c r="J4" t="n">
-        <v>1.866704778512724e-39</v>
+        <v>4.519620739491309e-40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -1207,24 +1851,24 @@
         <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>-14973.20514195754</v>
+        <v>-14988.99769465362</v>
       </c>
       <c r="I5" t="n">
-        <v>-15006.75933872866</v>
+        <v>-15011.369175805</v>
       </c>
       <c r="J5" t="n">
-        <v>8.510919941412981e-40</v>
+        <v>1.900336117676957e-46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -1236,21 +1880,21 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>-14943.23147094551</v>
+        <v>-14987.37536665711</v>
       </c>
       <c r="I6" t="n">
-        <v>-14965.59083699425</v>
+        <v>-15026.51839866134</v>
       </c>
       <c r="J6" t="n">
-        <v>6.38992595631588e-13</v>
+        <v>1.01197208250074e-37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1271,13 +1915,13 @@
         <v>7</v>
       </c>
       <c r="H7" t="n">
-        <v>-14939.49996013833</v>
+        <v>-14942.88332731705</v>
       </c>
       <c r="I7" t="n">
-        <v>-14967.44663925419</v>
+        <v>-14965.24269336578</v>
       </c>
       <c r="J7" t="n">
-        <v>7.441604599095469e-10</v>
+        <v>2.808135994134758e-12</v>
       </c>
     </row>
     <row r="8">
@@ -1303,13 +1947,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="n">
-        <v>-14939.08949682555</v>
+        <v>-14937.80897366612</v>
       </c>
       <c r="I8" t="n">
-        <v>-14967.03617594141</v>
+        <v>-14965.75565278197</v>
       </c>
       <c r="J8" t="n">
-        <v>4.710386713303525e-10</v>
+        <v>2.418673602880404e-09</v>
       </c>
     </row>
     <row r="9">
@@ -1320,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -1332,16 +1976,16 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H9" t="n">
-        <v>-14937.50244910685</v>
+        <v>-14930.49232897428</v>
       </c>
       <c r="I9" t="n">
-        <v>-14965.46427974945</v>
+        <v>-14964.0283439133</v>
       </c>
       <c r="J9" t="n">
-        <v>2.379334705431504e-59</v>
+        <v>1.957779017213172e-09</v>
       </c>
     </row>
     <row r="10">
@@ -1367,13 +2011,13 @@
         <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>-14924.05355433935</v>
+        <v>-14925.73982469697</v>
       </c>
       <c r="I10" t="n">
-        <v>-14957.5865336092</v>
+        <v>-14959.27280396682</v>
       </c>
       <c r="J10" t="n">
-        <v>4.942986675302808e-10</v>
+        <v>6.856733101164526e-10</v>
       </c>
     </row>
     <row r="11">
@@ -1384,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -1399,13 +2043,13 @@
         <v>7</v>
       </c>
       <c r="H11" t="n">
-        <v>-14913.08768112344</v>
+        <v>-14913.9958028526</v>
       </c>
       <c r="I11" t="n">
-        <v>-14946.62369606247</v>
+        <v>-14953.11761200075</v>
       </c>
       <c r="J11" t="n">
-        <v>7.53560107204444e-11</v>
+        <v>3.154031886817702e-06</v>
       </c>
     </row>
   </sheetData>
@@ -1414,6 +2058,75 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>activo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_recomendado</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>BIC_recomendado</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_alternativo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ΔBIC_alt_vs_best</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ARIMA(3,1,1)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>-15808.93391855776</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>SARIMA(2,0,0)x(1,1,1)[5]</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>803.9339715510978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1438,15 +2151,13 @@
       <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">EURUSD (diario)
-• Periodo: 2018-01-22 00:00:00 → 2025-10-03 00:00:00
-• Precio medio: 1.1195 | Último: 1.1739 | Rango [0.95906, 1.25068]
-• Riesgo (log-returns): σ=0.0046 (~0.46%), VaR95=-0.73%, ES95=-0.98%, JB p=3.9e-54 ⇒ no normal.
+• Periodo: 2018-01-23 00:00:00 → 2025-10-06 00:00:00
+• Precio medio: 1.1195 | Último: 1.1712799999999999 | Rango [0.95906, 1.25068]
+• Riesgo (log-returns): σ=0.0046 (~0.46%), VaR95=-0.73%, ES95=-0.98%, JB p=3.2e-54 ⇒ no normal.
 • MDD aprox.: -23.32%.
-• Modelo recomendado (por BIC): ARIMA(2,1,1)
-  - d: nº de diferencias sobre log-precio (quita tendencia).
-  - p: memoria AR en retornos (lags de la serie diferenciada).
-  - q: media móvil (impacto de shocks previos en el error).
-  - Diagnóstico deseable: Ljung–Box p ≥ 0.05 en residuales (ruido blanco).
+• Modelo recomendado (menor BIC): ARIMA(3,1,1)  | BIC=-15808.93, AIC=-15836.93, Ljung–Box p=0.44609863572287267.
+  Alternativa: SARIMA(2,0,0)x(1,1,1)[5]  | BIC=-15005.00 (ΔBIC=+803.93).
+  Diagnóstico esperado: residuales ≈ ruido blanco (Ljung–Box p≥0.05) y ACF/PACF de residuales sin picos significativos.
 </t>
         </is>
       </c>
@@ -1456,7 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1495,7 +2206,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>51.7 (neutral)</t>
+          <t>49.0 (neutral)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1509,13 +2220,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1526,307 +2237,187 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Sección</t>
+          <t>check</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Columna</t>
+          <t>metric</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Significado</t>
+          <t>value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ARIMA_candidates</t>
+          <t>shape</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>p,d,q</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Órdenes no estacionales: AR (p), diferencias (d), MA (q).</t>
-        </is>
+          <t>rows</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ARIMA_candidates</t>
+          <t>shape</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>bic</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Criterio de información bayesiano (menor es mejor).</t>
-        </is>
+          <t>cols</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ARIMA_candidates</t>
+          <t>index</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>aic</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Criterio de Akaike (menor es mejor).</t>
-        </is>
+          <t>is_datetimeindex</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ARIMA_candidates</t>
+          <t>index</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>lb_p</t>
+          <t>tzinfo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>p-value de Ljung–Box en residuales (≥0.05 sugiere ruido blanco).</t>
+          <t>naive</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SARIMA_candidates</t>
+          <t>duplicates</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>p,d,q</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Parte no estacional del modelo.</t>
-        </is>
+          <t>rows_duplicated</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SARIMA_candidates</t>
+          <t>gaps</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P,D,Q</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Parte estacional del modelo (lags a múltiplos de s).</t>
-        </is>
+          <t>n_missing_timestamps</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SARIMA_candidates</t>
+          <t>gaps</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>missing_preview</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Periodo estacional (diario: 5=semana hábil, 7=semana calendario).</t>
+          <t>2018-01-27, 2018-01-28, 2018-02-03, ..., 2025-09-28, 2025-10-04, 2025-10-05</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SARIMA_candidates</t>
+          <t>price_checks</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>bic,aic,lb_p</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Mismos criterios que en ARIMA.</t>
-        </is>
+          <t>n_nan_price</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STATS</t>
+          <t>price_checks</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>mean,std</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Media y desviación típica diaria de log-returns.</t>
-        </is>
+          <t>n_nonpositive</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>STATS</t>
+          <t>volume_checks</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>skew,kurtosis</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Asimetría y exceso de curtosis (colas).</t>
-        </is>
+          <t>n_nan_volume</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>STATS</t>
+          <t>volume_checks</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>JB_stat,JB_pvalue</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Test de normalidad Jarque–Bera (p&lt;0.05 ⇒ no normal).</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>STATS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>VaR_95,ES_95</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Pérdida al 95% y pérdida media condicional en el 5% peor.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>RESUMEN</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>precio_ultimo/promedio/min/max</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Niveles de precio del periodo resampleado.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>RESUMEN</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>inicio,fin,filas</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Fechas de cobertura y nº de barras.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Signals_guide</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Tendencia_MA</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Cruce SMA50 vs SMA200 (lectura descriptiva).</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Signals_guide</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>RSI_14</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Sobrecompra/sobreventa/neutral (14).</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Signals_guide</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>MACD</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Relación MACD vs señal (12,26,9).</t>
-        </is>
+          <t>n_zero_volume</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza modelo ARIMA y Backtesting
</commit_message>
<xml_diff>
--- a/outputs/eda/EDA_informe.xlsx
+++ b/outputs/eda/EDA_informe.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="EURUSD_HEAD" sheetId="1" state="visible" r:id="rId1"/>
@@ -28,12 +27,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -50,12 +57,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -68,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -77,13 +99,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -448,7 +469,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -487,107 +508,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>43123</v>
+      <c r="A2" s="2" t="n">
+        <v>43133</v>
       </c>
       <c r="B2" t="n">
-        <v>1.22606</v>
+        <v>1.25075</v>
       </c>
       <c r="C2" t="n">
-        <v>1.23062</v>
+        <v>1.2518</v>
       </c>
       <c r="D2" t="n">
-        <v>1.22228</v>
+        <v>1.24089</v>
       </c>
       <c r="E2" t="n">
-        <v>1.22979</v>
+        <v>1.24547</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>43124</v>
+      <c r="A3" s="2" t="n">
+        <v>43136</v>
       </c>
       <c r="B3" t="n">
-        <v>1.22983</v>
+        <v>1.24348</v>
       </c>
       <c r="C3" t="n">
-        <v>1.24147</v>
+        <v>1.24747</v>
       </c>
       <c r="D3" t="n">
-        <v>1.229</v>
+        <v>1.23624</v>
       </c>
       <c r="E3" t="n">
-        <v>1.24069</v>
+        <v>1.23663</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
-        <v>43125</v>
+      <c r="A4" s="2" t="n">
+        <v>43137</v>
       </c>
       <c r="B4" t="n">
-        <v>1.24071</v>
+        <v>1.2366</v>
       </c>
       <c r="C4" t="n">
-        <v>1.25376</v>
+        <v>1.24344</v>
       </c>
       <c r="D4" t="n">
-        <v>1.23638</v>
+        <v>1.23136</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23969</v>
+        <v>1.23763</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
-        <v>43126</v>
+      <c r="A5" s="2" t="n">
+        <v>43138</v>
       </c>
       <c r="B5" t="n">
-        <v>1.23926</v>
+        <v>1.23761</v>
       </c>
       <c r="C5" t="n">
-        <v>1.24935</v>
+        <v>1.24059</v>
       </c>
       <c r="D5" t="n">
-        <v>1.23698</v>
+        <v>1.22458</v>
       </c>
       <c r="E5" t="n">
-        <v>1.24273</v>
+        <v>1.22644</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
-        <v>43129</v>
+      <c r="A6" s="2" t="n">
+        <v>43139</v>
       </c>
       <c r="B6" t="n">
-        <v>1.24235</v>
+        <v>1.22619</v>
       </c>
       <c r="C6" t="n">
-        <v>1.2432</v>
+        <v>1.22949</v>
       </c>
       <c r="D6" t="n">
-        <v>1.23366</v>
+        <v>1.22119</v>
       </c>
       <c r="E6" t="n">
-        <v>1.23827</v>
+        <v>1.22464</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -606,57 +627,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>series</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>stat</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>pvalue</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>lags_used</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>nobs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>crit_1%</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>crit_5%</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>crit_10%</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>conclusion</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>crit_2.5%</t>
         </is>
@@ -674,10 +695,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-2.385964301215576</v>
+        <v>-2.571946055209313</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1457371306121847</v>
+        <v>0.09893516712107148</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -713,7 +734,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2.035311725137694</v>
+        <v>1.948219142628974</v>
       </c>
       <c r="D3" t="n">
         <v>0.01</v>
@@ -752,7 +773,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-44.3669005477752</v>
+        <v>-44.35429403033181</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -791,7 +812,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1766043103880247</v>
+        <v>0.1915055999534681</v>
       </c>
       <c r="D5" t="n">
         <v>0.1</v>
@@ -838,17 +859,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>lb_p_10</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>lb_p_20</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>modelo</t>
         </is>
@@ -856,10 +877,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9998647612658635</v>
+        <v>0.9999821503832312</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9999999870973478</v>
+        <v>0.9999999998654038</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -887,17 +908,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Sección</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Columna</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Significado</t>
         </is>
@@ -1296,17 +1317,17 @@
       <c r="B2" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>43123</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>45936</v>
+      <c r="C2" s="3" t="n">
+        <v>43133</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>45946</v>
       </c>
       <c r="E2" t="n">
-        <v>1.17128</v>
+        <v>1.16672</v>
       </c>
       <c r="F2" t="n">
-        <v>1.119474055</v>
+        <v>1.11916028</v>
       </c>
       <c r="G2" t="n">
         <v>0.95906</v>
@@ -1316,7 +1337,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1386,22 +1407,22 @@
         <v>1999</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.438532025893065e-05</v>
+        <v>-3.26746251374379e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004578956744010433</v>
+        <v>0.004576920850448997</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0995152332483944</v>
+        <v>0.09890844871594479</v>
       </c>
       <c r="E2" t="n">
-        <v>1.715642934253303</v>
+        <v>1.717128146346002</v>
       </c>
       <c r="F2" t="n">
-        <v>246.3792003493377</v>
+        <v>246.760940223135</v>
       </c>
       <c r="G2" t="n">
-        <v>3.158176635593929e-54</v>
+        <v>2.609412003949872e-54</v>
       </c>
       <c r="H2" t="n">
         <v>-0.007311072280727136</v>
@@ -1411,7 +1432,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1430,32 +1451,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>q</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>bic</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>aic</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>lb_p</t>
         </is>
@@ -1472,13 +1493,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-15808.93391855776</v>
+        <v>-15800.77762366929</v>
       </c>
       <c r="E2" t="n">
-        <v>-15836.9334283538</v>
+        <v>-15828.77713346534</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4460986357228727</v>
+        <v>0.1000060418621142</v>
       </c>
     </row>
     <row r="3">
@@ -1492,18 +1513,18 @@
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>-15771.5833113377</v>
+        <v>-15799.75747787519</v>
       </c>
       <c r="E3" t="n">
-        <v>-15805.18272309296</v>
+        <v>-15833.35688963044</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0008960997602847229</v>
+        <v>0.2245264713412904</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1512,18 +1533,18 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>-15722.58449386945</v>
+        <v>-15761.90182219796</v>
       </c>
       <c r="E4" t="n">
-        <v>-15744.98410170628</v>
+        <v>-15801.10113591242</v>
       </c>
       <c r="F4" t="n">
-        <v>8.99773815128505e-07</v>
+        <v>0.004093998112323158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -1532,18 +1553,18 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>-15687.65715511697</v>
+        <v>-15739.7968573709</v>
       </c>
       <c r="E5" t="n">
-        <v>-15715.65666491301</v>
+        <v>-15762.19646520773</v>
       </c>
       <c r="F5" t="n">
-        <v>9.057281081856922e-07</v>
+        <v>0.0001972967494500679</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -1552,13 +1573,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>-15661.53036690277</v>
+        <v>-15692.4763790029</v>
       </c>
       <c r="E6" t="n">
-        <v>-15700.72968061723</v>
+        <v>-15720.47588879894</v>
       </c>
       <c r="F6" t="n">
-        <v>1.544201155603525e-06</v>
+        <v>8.597180351793514e-07</v>
       </c>
     </row>
     <row r="7">
@@ -1572,13 +1593,13 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>-15650.35349427511</v>
+        <v>-15653.02218413727</v>
       </c>
       <c r="E7" t="n">
-        <v>-15667.15320015274</v>
+        <v>-15669.8218900149</v>
       </c>
       <c r="F7" t="n">
-        <v>8.88755867228312e-09</v>
+        <v>6.903797625439893e-09</v>
       </c>
     </row>
     <row r="8">
@@ -1589,21 +1610,21 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>-15629.44824767751</v>
+        <v>-15642.94339543019</v>
       </c>
       <c r="E8" t="n">
-        <v>-15657.44775747356</v>
+        <v>-15665.34300326703</v>
       </c>
       <c r="F8" t="n">
-        <v>1.075416108568944e-08</v>
+        <v>1.983240399087305e-10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1612,18 +1633,18 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>-15626.22450793347</v>
+        <v>-15632.27738177508</v>
       </c>
       <c r="E9" t="n">
-        <v>-15648.62411577031</v>
+        <v>-15660.27689157112</v>
       </c>
       <c r="F9" t="n">
-        <v>6.62281654959856e-09</v>
+        <v>8.084745218880163e-09</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -1632,33 +1653,33 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>-15608.86063372448</v>
+        <v>-15628.77573629129</v>
       </c>
       <c r="E10" t="n">
-        <v>-15642.46004547973</v>
+        <v>-15651.17534412813</v>
       </c>
       <c r="F10" t="n">
-        <v>3.798487396284246e-09</v>
+        <v>5.139020514759784e-09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
       <c r="D11" t="n">
-        <v>-15551.64212938027</v>
+        <v>-15610.92945870039</v>
       </c>
       <c r="E11" t="n">
-        <v>-15574.0417372171</v>
+        <v>-15644.52887045564</v>
       </c>
       <c r="F11" t="n">
-        <v>2.896334386935552e-14</v>
+        <v>2.599178345878544e-09</v>
       </c>
     </row>
   </sheetData>
@@ -1681,52 +1702,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>q</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Q</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>bic</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>aic</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>lb_p</t>
         </is>
@@ -1755,13 +1776,13 @@
         <v>5</v>
       </c>
       <c r="H2" t="n">
-        <v>-15004.99994700666</v>
+        <v>-15004.13992403393</v>
       </c>
       <c r="I2" t="n">
-        <v>-15032.96177764926</v>
+        <v>-15032.10175467653</v>
       </c>
       <c r="J2" t="n">
-        <v>3.43786698747402e-41</v>
+        <v>6.201472539987862e-39</v>
       </c>
     </row>
     <row r="3">
@@ -1772,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -1787,13 +1808,13 @@
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>-15002.94368122421</v>
+        <v>-14999.61426603795</v>
       </c>
       <c r="I3" t="n">
-        <v>-15030.90551186681</v>
+        <v>-15021.98574718933</v>
       </c>
       <c r="J3" t="n">
-        <v>2.371123554633866e-41</v>
+        <v>1.496041590341463e-46</v>
       </c>
     </row>
     <row r="4">
@@ -1804,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1819,24 +1840,24 @@
         <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>-14993.59098211363</v>
+        <v>-14999.42846275214</v>
       </c>
       <c r="I4" t="n">
-        <v>-15027.14215240297</v>
+        <v>-15027.39029339474</v>
       </c>
       <c r="J4" t="n">
-        <v>4.519620739491309e-40</v>
+        <v>2.855441840545584e-38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -1851,18 +1872,18 @@
         <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>-14988.99769465362</v>
+        <v>-14995.27368496538</v>
       </c>
       <c r="I5" t="n">
-        <v>-15011.369175805</v>
+        <v>-15028.8278817365</v>
       </c>
       <c r="J5" t="n">
-        <v>1.900336117676957e-46</v>
+        <v>9.905196451179608e-39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1883,24 +1904,24 @@
         <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>-14987.37536665711</v>
+        <v>-14992.51848732785</v>
       </c>
       <c r="I6" t="n">
-        <v>-15026.51839866134</v>
+        <v>-15026.06965761719</v>
       </c>
       <c r="J6" t="n">
-        <v>1.01197208250074e-37</v>
+        <v>1.793666234272783e-38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -1912,16 +1933,16 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>-14942.88332731705</v>
+        <v>-14987.74745971975</v>
       </c>
       <c r="I7" t="n">
-        <v>-14965.24269336578</v>
+        <v>-15026.89049172398</v>
       </c>
       <c r="J7" t="n">
-        <v>2.808135994134758e-12</v>
+        <v>5.293977344268944e-38</v>
       </c>
     </row>
     <row r="8">
@@ -1932,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -1947,13 +1968,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="n">
-        <v>-14937.80897366612</v>
+        <v>-14946.82024742134</v>
       </c>
       <c r="I8" t="n">
-        <v>-14965.75565278197</v>
+        <v>-14969.17961347007</v>
       </c>
       <c r="J8" t="n">
-        <v>2.418673602880404e-09</v>
+        <v>2.378169138662052e-11</v>
       </c>
     </row>
     <row r="9">
@@ -1964,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -1979,13 +2000,13 @@
         <v>7</v>
       </c>
       <c r="H9" t="n">
-        <v>-14930.49232897428</v>
+        <v>-14942.68680235657</v>
       </c>
       <c r="I9" t="n">
-        <v>-14964.0283439133</v>
+        <v>-14970.63348147243</v>
       </c>
       <c r="J9" t="n">
-        <v>1.957779017213172e-09</v>
+        <v>1.856127527514104e-09</v>
       </c>
     </row>
     <row r="10">
@@ -1996,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -2011,18 +2032,18 @@
         <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>-14925.73982469697</v>
+        <v>-14942.27510058138</v>
       </c>
       <c r="I10" t="n">
-        <v>-14959.27280396682</v>
+        <v>-14970.22177969723</v>
       </c>
       <c r="J10" t="n">
-        <v>6.856733101164526e-10</v>
+        <v>1.971369269602338e-09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -2043,13 +2064,13 @@
         <v>7</v>
       </c>
       <c r="H11" t="n">
-        <v>-14913.9958028526</v>
+        <v>-14924.61587472576</v>
       </c>
       <c r="I11" t="n">
-        <v>-14953.11761200075</v>
+        <v>-14958.1488539956</v>
       </c>
       <c r="J11" t="n">
-        <v>3.154031886817702e-06</v>
+        <v>8.44736018330489e-11</v>
       </c>
     </row>
   </sheetData>
@@ -2072,27 +2093,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>modelo_recomendado</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>BIC_recomendado</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>modelo_alternativo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>ΔBIC_alt_vs_best</t>
         </is>
@@ -2110,7 +2131,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-15808.93391855776</v>
+        <v>-15800.77762366929</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -2118,7 +2139,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>803.9339715510978</v>
+        <v>796.6376996353647</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2162,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Narrativa</t>
         </is>
@@ -2151,12 +2172,12 @@
       <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">EURUSD (diario)
-• Periodo: 2018-01-23 00:00:00 → 2025-10-06 00:00:00
-• Precio medio: 1.1195 | Último: 1.1712799999999999 | Rango [0.95906, 1.25068]
-• Riesgo (log-returns): σ=0.0046 (~0.46%), VaR95=-0.73%, ES95=-0.98%, JB p=3.2e-54 ⇒ no normal.
+• Periodo: 2018-02-02 00:00:00 → 2025-10-16 00:00:00
+• Precio medio: 1.1192 | Último: 1.16672 | Rango [0.95906, 1.25068]
+• Riesgo (log-returns): σ=0.0046 (~0.46%), VaR95=-0.73%, ES95=-0.98%, JB p=2.6e-54 ⇒ no normal.
 • MDD aprox.: -23.32%.
-• Modelo recomendado (menor BIC): ARIMA(3,1,1)  | BIC=-15808.93, AIC=-15836.93, Ljung–Box p=0.44609863572287267.
-  Alternativa: SARIMA(2,0,0)x(1,1,1)[5]  | BIC=-15005.00 (ΔBIC=+803.93).
+• Modelo recomendado (menor BIC): ARIMA(3,1,1)  | BIC=-15800.78, AIC=-15828.78, Ljung–Box p=0.10000604186211419.
+  Alternativa: SARIMA(2,0,0)x(1,1,1)[5]  | BIC=-15004.14 (ΔBIC=+796.64).
   Diagnóstico esperado: residuales ≈ ruido blanco (Ljung–Box p≥0.05) y ACF/PACF de residuales sin picos significativos.
 </t>
         </is>
@@ -2182,17 +2203,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Tendencia_MA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>RSI_14</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>MACD</t>
         </is>
@@ -2235,17 +2256,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>check</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>metric</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -2356,7 +2377,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2018-01-27, 2018-01-28, 2018-02-03, ..., 2025-09-28, 2025-10-04, 2025-10-05</t>
+          <t>2018-02-03, 2018-02-04, 2018-02-10, ..., 2025-10-05, 2025-10-11, 2025-10-12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agregan los demás modelos junto con las métricas, además del reporte unificado
</commit_message>
<xml_diff>
--- a/outputs/eda/EDA_informe.xlsx
+++ b/outputs/eda/EDA_informe.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="EURUSD_HEAD" sheetId="1" state="visible" r:id="rId1"/>
@@ -27,20 +28,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -57,27 +50,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -90,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -99,12 +77,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -469,7 +448,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -508,107 +487,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>43133</v>
+      <c r="A2" s="4" t="n">
+        <v>45786.95833333334</v>
       </c>
       <c r="B2" t="n">
-        <v>1.25075</v>
+        <v>1.12566</v>
       </c>
       <c r="C2" t="n">
-        <v>1.2518</v>
+        <v>1.12567</v>
       </c>
       <c r="D2" t="n">
-        <v>1.24089</v>
+        <v>1.12467</v>
       </c>
       <c r="E2" t="n">
-        <v>1.24547</v>
+        <v>1.12475</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>43136</v>
+      <c r="A3" s="4" t="n">
+        <v>45789</v>
       </c>
       <c r="B3" t="n">
-        <v>1.24348</v>
+        <v>1.1192</v>
       </c>
       <c r="C3" t="n">
-        <v>1.24747</v>
+        <v>1.12223</v>
       </c>
       <c r="D3" t="n">
-        <v>1.23624</v>
+        <v>1.1192</v>
       </c>
       <c r="E3" t="n">
-        <v>1.23663</v>
+        <v>1.12093</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>43137</v>
+      <c r="A4" s="4" t="n">
+        <v>45789.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>1.2366</v>
+        <v>1.12092</v>
       </c>
       <c r="C4" t="n">
-        <v>1.24344</v>
+        <v>1.12308</v>
       </c>
       <c r="D4" t="n">
-        <v>1.23136</v>
+        <v>1.12061</v>
       </c>
       <c r="E4" t="n">
-        <v>1.23763</v>
+        <v>1.12246</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>43138</v>
+      <c r="A5" s="4" t="n">
+        <v>45789.08333333334</v>
       </c>
       <c r="B5" t="n">
-        <v>1.23761</v>
+        <v>1.12245</v>
       </c>
       <c r="C5" t="n">
-        <v>1.24059</v>
+        <v>1.12355</v>
       </c>
       <c r="D5" t="n">
-        <v>1.22458</v>
+        <v>1.12226</v>
       </c>
       <c r="E5" t="n">
-        <v>1.22644</v>
+        <v>1.12276</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>43139</v>
+      <c r="A6" s="4" t="n">
+        <v>45789.125</v>
       </c>
       <c r="B6" t="n">
-        <v>1.22619</v>
+        <v>1.12276</v>
       </c>
       <c r="C6" t="n">
-        <v>1.22949</v>
+        <v>1.12387</v>
       </c>
       <c r="D6" t="n">
-        <v>1.22119</v>
+        <v>1.12245</v>
       </c>
       <c r="E6" t="n">
-        <v>1.22464</v>
+        <v>1.12381</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -627,57 +606,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>series</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>stat</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>pvalue</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>lags_used</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>nobs</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>crit_1%</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>crit_5%</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>crit_10%</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>conclusion</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>crit_2.5%</t>
         </is>
@@ -695,25 +674,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-2.571946055209313</v>
+        <v>-2.500673159142389</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09893516712107148</v>
+        <v>0.1153106237735516</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>1999</v>
+        <v>2995</v>
       </c>
       <c r="G2" t="n">
-        <v>-3.433625496286504</v>
+        <v>-3.432535279976574</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.862986937508278</v>
+        <v>-2.862505515243151</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.567540287745173</v>
+        <v>-2.567283969247578</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -734,13 +713,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.948219142628974</v>
+        <v>4.326385467667958</v>
       </c>
       <c r="D3" t="n">
         <v>0.01</v>
       </c>
       <c r="E3" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
@@ -773,25 +752,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-44.35429403033181</v>
+        <v>-27.93437967753166</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>1998</v>
+        <v>2995</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.433627137787501</v>
+        <v>-3.432535279976574</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.862987662236822</v>
+        <v>-2.862505515243151</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.56754067362658</v>
+        <v>-2.567283969247578</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -812,13 +791,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1915055999534681</v>
+        <v>0.1728328717674746</v>
       </c>
       <c r="D5" t="n">
         <v>0.1</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
@@ -859,17 +838,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>lb_p_10</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>lb_p_20</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>modelo</t>
         </is>
@@ -877,14 +856,14 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9999821503832312</v>
+        <v>0.9999999999347068</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9999999998654038</v>
+        <v>0.9999999999999321</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ARIMA(3,1,1)</t>
+          <t>ARIMA(0,1,3)</t>
         </is>
       </c>
     </row>
@@ -908,17 +887,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Sección</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Columna</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Significado</t>
         </is>
@@ -1315,29 +1294,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>43133</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>45946</v>
+        <v>3000</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>45786.95833333334</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>45961.91666666666</v>
       </c>
       <c r="E2" t="n">
-        <v>1.16672</v>
+        <v>1.15363</v>
       </c>
       <c r="F2" t="n">
-        <v>1.11916028</v>
+        <v>1.159837796666667</v>
       </c>
       <c r="G2" t="n">
-        <v>0.95906</v>
+        <v>1.10787</v>
       </c>
       <c r="H2" t="n">
-        <v>1.25068</v>
+        <v>1.18705</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1404,35 +1383,35 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1999</v>
+        <v>2999</v>
       </c>
       <c r="B2" t="n">
-        <v>-3.26746251374379e-05</v>
+        <v>8.453719246120297e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004576920850448997</v>
+        <v>0.0009369278788371978</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09890844871594479</v>
+        <v>0.6512681585161567</v>
       </c>
       <c r="E2" t="n">
-        <v>1.717128146346002</v>
+        <v>22.34552008303871</v>
       </c>
       <c r="F2" t="n">
-        <v>246.760940223135</v>
+        <v>62387.34024526915</v>
       </c>
       <c r="G2" t="n">
-        <v>2.609412003949872e-54</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.007311072280727136</v>
+        <v>-0.00132615853813165</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.009813679026569542</v>
+        <v>-0.002083084943351822</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1451,32 +1430,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>q</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>bic</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>aic</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>lb_p</t>
         </is>
@@ -1484,27 +1463,27 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
       <c r="D2" t="n">
-        <v>-15800.77762366929</v>
+        <v>-33124.18313415989</v>
       </c>
       <c r="E2" t="n">
-        <v>-15828.77713346534</v>
+        <v>-33148.20593687454</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1000060418621142</v>
+        <v>3.424488788078203e-07</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -1513,18 +1492,18 @@
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>-15799.75747787519</v>
+        <v>-33113.25942538794</v>
       </c>
       <c r="E3" t="n">
-        <v>-15833.35688963044</v>
+        <v>-33155.29933013857</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2245264713412904</v>
+        <v>1.92775369572879e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -1533,18 +1512,18 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>-15761.90182219796</v>
+        <v>-33082.33835318684</v>
       </c>
       <c r="E4" t="n">
-        <v>-15801.10113591242</v>
+        <v>-33118.37255725882</v>
       </c>
       <c r="F4" t="n">
-        <v>0.004093998112323158</v>
+        <v>2.430525803501257e-06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -1553,33 +1532,33 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>-15739.7968573709</v>
+        <v>-33070.45351493863</v>
       </c>
       <c r="E5" t="n">
-        <v>-15762.19646520773</v>
+        <v>-33100.48201833194</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0001972967494500679</v>
+        <v>1.151196518178958e-08</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>-15692.4763790029</v>
+        <v>-33017.28739710082</v>
       </c>
       <c r="E6" t="n">
-        <v>-15720.47588879894</v>
+        <v>-33053.32160117279</v>
       </c>
       <c r="F6" t="n">
-        <v>8.597180351793514e-07</v>
+        <v>4.069418252615827e-12</v>
       </c>
     </row>
     <row r="7">
@@ -1593,33 +1572,33 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>-15653.02218413727</v>
+        <v>-33015.53087457013</v>
       </c>
       <c r="E7" t="n">
-        <v>-15669.8218900149</v>
+        <v>-33033.54797660612</v>
       </c>
       <c r="F7" t="n">
-        <v>6.903797625439893e-09</v>
+        <v>2.562747194854149e-13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
       <c r="D8" t="n">
-        <v>-15642.94339543019</v>
+        <v>-33000.13556181392</v>
       </c>
       <c r="E8" t="n">
-        <v>-15665.34300326703</v>
+        <v>-33024.15836452857</v>
       </c>
       <c r="F8" t="n">
-        <v>1.983240399087305e-10</v>
+        <v>6.72064970592772e-16</v>
       </c>
     </row>
     <row r="9">
@@ -1633,53 +1612,53 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>-15632.27738177508</v>
+        <v>-32964.15639933311</v>
       </c>
       <c r="E9" t="n">
-        <v>-15660.27689157112</v>
+        <v>-32994.18490272642</v>
       </c>
       <c r="F9" t="n">
-        <v>8.084745218880163e-09</v>
+        <v>1.035133966662409e-14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>-15628.77573629129</v>
+        <v>-32927.36234988436</v>
       </c>
       <c r="E10" t="n">
-        <v>-15651.17534412813</v>
+        <v>-32939.37375124168</v>
       </c>
       <c r="F10" t="n">
-        <v>5.139020514759784e-09</v>
+        <v>1.189593933848645e-20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-15610.92945870039</v>
+        <v>-32840.07674584557</v>
       </c>
       <c r="E11" t="n">
-        <v>-15644.52887045564</v>
+        <v>-32858.09384788155</v>
       </c>
       <c r="F11" t="n">
-        <v>2.599178345878544e-09</v>
+        <v>1.062238414749708e-22</v>
       </c>
     </row>
   </sheetData>
@@ -1702,52 +1681,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>p</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>q</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Q</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>bic</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>aic</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>lb_p</t>
         </is>
@@ -1761,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -1776,13 +1755,13 @@
         <v>5</v>
       </c>
       <c r="H2" t="n">
-        <v>-15004.13992403393</v>
+        <v>-31672.97414445043</v>
       </c>
       <c r="I2" t="n">
-        <v>-15032.10175467653</v>
+        <v>-31714.9765909177</v>
       </c>
       <c r="J2" t="n">
-        <v>6.201472539987862e-39</v>
+        <v>2.049932764840596e-117</v>
       </c>
     </row>
     <row r="3">
@@ -1793,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -1808,27 +1787,27 @@
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>-14999.61426603795</v>
+        <v>-31395.34245308244</v>
       </c>
       <c r="I3" t="n">
-        <v>-15021.98574718933</v>
+        <v>-31425.34420055906</v>
       </c>
       <c r="J3" t="n">
-        <v>1.496041590341463e-46</v>
+        <v>8.043060828668412e-150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -1837,30 +1816,30 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H4" t="n">
-        <v>-14999.42846275214</v>
+        <v>-31364.10450137254</v>
       </c>
       <c r="I4" t="n">
-        <v>-15027.39029339474</v>
+        <v>-31388.10053022551</v>
       </c>
       <c r="J4" t="n">
-        <v>2.855441840545584e-38</v>
+        <v>7.331380521135604e-128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -1872,18 +1851,18 @@
         <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>-14995.27368496538</v>
+        <v>-31362.10736544289</v>
       </c>
       <c r="I5" t="n">
-        <v>-15028.8278817365</v>
+        <v>-31380.11042532686</v>
       </c>
       <c r="J5" t="n">
-        <v>9.905196451179608e-39</v>
+        <v>4.338603983964221e-135</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1892,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -1904,27 +1883,27 @@
         <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>-14992.51848732785</v>
+        <v>-31349.94648027984</v>
       </c>
       <c r="I6" t="n">
-        <v>-15026.06965761719</v>
+        <v>-31385.94857725179</v>
       </c>
       <c r="J6" t="n">
-        <v>1.793666234272783e-38</v>
+        <v>4.11614979928951e-148</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -1933,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H7" t="n">
-        <v>-14987.74745971975</v>
+        <v>-31317.46697656145</v>
       </c>
       <c r="I7" t="n">
-        <v>-15026.89049172398</v>
+        <v>-31341.46166200552</v>
       </c>
       <c r="J7" t="n">
-        <v>5.293977344268944e-38</v>
+        <v>1.296112884029828e-144</v>
       </c>
     </row>
     <row r="8">
@@ -1956,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -1968,13 +1947,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="n">
-        <v>-14946.82024742134</v>
+        <v>-31303.05180785679</v>
       </c>
       <c r="I8" t="n">
-        <v>-14969.17961347007</v>
+        <v>-31321.04882949653</v>
       </c>
       <c r="J8" t="n">
-        <v>2.378169138662052e-11</v>
+        <v>3.650890951398039e-135</v>
       </c>
     </row>
     <row r="9">
@@ -1985,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -2000,18 +1979,18 @@
         <v>7</v>
       </c>
       <c r="H9" t="n">
-        <v>-14942.68680235657</v>
+        <v>-31047.42836645367</v>
       </c>
       <c r="I9" t="n">
-        <v>-14970.63348147243</v>
+        <v>-31083.42039461977</v>
       </c>
       <c r="J9" t="n">
-        <v>1.856127527514104e-09</v>
+        <v>6.794778950429056e-68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -2020,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -2029,16 +2008,16 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>-14942.27510058138</v>
+        <v>-30778.83133393817</v>
       </c>
       <c r="I10" t="n">
-        <v>-14970.22177969723</v>
+        <v>-30808.83475786075</v>
       </c>
       <c r="J10" t="n">
-        <v>1.971369269602338e-09</v>
+        <v>8.149620897596561e-163</v>
       </c>
     </row>
     <row r="11">
@@ -2049,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -2061,16 +2040,16 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="n">
-        <v>-14924.61587472576</v>
+        <v>-30774.14714315169</v>
       </c>
       <c r="I11" t="n">
-        <v>-14958.1488539956</v>
+        <v>-30798.14988228975</v>
       </c>
       <c r="J11" t="n">
-        <v>8.44736018330489e-11</v>
+        <v>3.802182991198937e-126</v>
       </c>
     </row>
   </sheetData>
@@ -2093,27 +2072,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>activo</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>modelo_recomendado</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>BIC_recomendado</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>modelo_alternativo</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ΔBIC_alt_vs_best</t>
         </is>
@@ -2127,19 +2106,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ARIMA(3,1,1)</t>
+          <t>ARIMA(0,1,3)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-15800.77762366929</v>
+        <v>-33124.18313415989</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SARIMA(2,0,0)x(1,1,1)[5]</t>
+          <t>SARIMA(2,0,2)x(1,1,1)[5]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>796.6376996353647</v>
+        <v>1451.208989709459</v>
       </c>
     </row>
   </sheetData>
@@ -2162,7 +2141,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Narrativa</t>
         </is>
@@ -2172,12 +2151,12 @@
       <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">EURUSD (diario)
-• Periodo: 2018-02-02 00:00:00 → 2025-10-16 00:00:00
-• Precio medio: 1.1192 | Último: 1.16672 | Rango [0.95906, 1.25068]
-• Riesgo (log-returns): σ=0.0046 (~0.46%), VaR95=-0.73%, ES95=-0.98%, JB p=2.6e-54 ⇒ no normal.
-• MDD aprox.: -23.32%.
-• Modelo recomendado (menor BIC): ARIMA(3,1,1)  | BIC=-15800.78, AIC=-15828.78, Ljung–Box p=0.10000604186211419.
-  Alternativa: SARIMA(2,0,0)x(1,1,1)[5]  | BIC=-15004.14 (ΔBIC=+796.64).
+• Periodo: 2025-05-09 23:00:00 → 2025-10-31 22:00:00
+• Precio medio: 1.1598 | Último: 1.15363 | Rango [1.10787, 1.18705]
+• Riesgo (log-returns): σ=0.0009 (~0.09%), VaR95=-0.13%, ES95=-0.21%, JB p=0 ⇒ no normal.
+• MDD aprox.: -6.67%.
+• Modelo recomendado (menor BIC): ARIMA(0,1,3)  | BIC=-33124.18, AIC=-33148.21, Ljung–Box p=3.424488788078203e-07.
+  Alternativa: SARIMA(2,0,2)x(1,1,1)[5]  | BIC=-31672.97 (ΔBIC=+1451.21).
   Diagnóstico esperado: residuales ≈ ruido blanco (Ljung–Box p≥0.05) y ACF/PACF de residuales sin picos significativos.
 </t>
         </is>
@@ -2203,17 +2182,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Tendencia_MA</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>RSI_14</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>MACD</t>
         </is>
@@ -2222,12 +2201,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alcista (SMA50&gt;SMA200)</t>
+          <t>Bajista (SMA50&lt;=SMA200)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>49.0 (neutral)</t>
+          <t>38.1 (neutral)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2256,17 +2235,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>check</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>metric</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -2284,7 +2263,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
@@ -2361,7 +2340,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>814</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="8">
@@ -2377,7 +2356,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2018-02-03, 2018-02-04, 2018-02-10, ..., 2025-10-05, 2025-10-11, 2025-10-12</t>
+          <t>2025-05-10 00:00:00, 2025-05-10 01:00:00, 2025-05-10 02:00:00, ..., 2025-10-26 21:00:00, 2025-10-26 22:00:00, 2025-10-26 23:00:00</t>
         </is>
       </c>
     </row>
@@ -2438,7 +2417,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>